<commit_message>
reading data from excel into hashmap
</commit_message>
<xml_diff>
--- a/Reading Data from Excel.xlsx
+++ b/Reading Data from Excel.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="testdata" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="sample" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="RestAssured" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="maoping" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="sample2" sheetId="4" r:id="rId7"/>
   </sheets>
@@ -14,9 +14,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>TestCase</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isbn </t>
+  </si>
+  <si>
+    <t>aisle</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rest AddBook </t>
+  </si>
+  <si>
+    <t xml:space="preserve">abcd </t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>Barman</t>
   </si>
   <si>
     <t xml:space="preserve">Name </t>
@@ -74,13 +98,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -110,11 +138,20 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -346,69 +383,69 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
+      <c r="B1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
+      <c r="A5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
+      <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -425,7 +462,42 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2">
+        <v>5765.0</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>

</xml_diff>